<commit_message>
Updated with Transparent Logo
Updated with Transparent Logo
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/Grade Card - Open.xlsx
+++ b/Batch 2018-20/Sem 1/Grade Card - Open.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1A4F50-5C67-4523-A859-1EF8C93E5392}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B71E0EE-9F9F-4916-86D6-0E3D8B47281F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
@@ -298,14 +298,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,7 +356,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -333,51 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,7 +426,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2148"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2146"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -29293,221 +29293,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="str">
+      <c r="A9" s="10" t="str">
         <f>"NAME OF THE CANDIDATE : "&amp;VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>NAME OF THE CANDIDATE : /ADIVAREKAR PRITI GIRIGHAR NAMRATA</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="str">
+      <c r="A11" s="10" t="str">
         <f>"HELD IN : "&amp;'[2]Subjects List'!$C$13</f>
         <v>HELD IN : JANUARY 2019</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="21" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="20" t="str">
+      <c r="B17" s="16" t="str">
         <f>'[2]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="3">
         <v>4</v>
       </c>
@@ -29531,12 +29531,12 @@
       <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="20" t="str">
+      <c r="B18" s="16" t="str">
         <f>'[2]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="3">
         <v>4</v>
       </c>
@@ -29560,12 +29560,12 @@
       <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="20" t="str">
+      <c r="B19" s="16" t="str">
         <f>'[2]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="3">
         <v>4</v>
       </c>
@@ -29589,12 +29589,12 @@
       <c r="A20" s="3">
         <v>4</v>
       </c>
-      <c r="B20" s="20" t="str">
+      <c r="B20" s="16" t="str">
         <f>'[2]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="3">
         <v>4</v>
       </c>
@@ -29618,12 +29618,12 @@
       <c r="A21" s="3">
         <v>5</v>
       </c>
-      <c r="B21" s="20" t="str">
+      <c r="B21" s="16" t="str">
         <f>'[2]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="3">
         <v>4</v>
       </c>
@@ -29647,12 +29647,12 @@
       <c r="A22" s="3">
         <v>6</v>
       </c>
-      <c r="B22" s="20" t="str">
+      <c r="B22" s="16" t="str">
         <f>'[2]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="3">
         <v>4</v>
       </c>
@@ -29676,12 +29676,12 @@
       <c r="A23" s="3">
         <v>7</v>
       </c>
-      <c r="B23" s="20" t="str">
+      <c r="B23" s="16" t="str">
         <f>'[2]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="3">
         <v>4</v>
       </c>
@@ -29705,12 +29705,12 @@
       <c r="A24" s="3">
         <v>8</v>
       </c>
-      <c r="B24" s="20" t="str">
+      <c r="B24" s="16" t="str">
         <f>'[2]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
       <c r="E24" s="3">
         <v>4</v>
       </c>
@@ -29732,11 +29732,11 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="5">
@@ -29750,43 +29750,43 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="str">
+      <c r="A26" s="22" t="str">
         <f>"Remark    :  "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BM$122,65,0)</f>
         <v>Remark    :  Unsuccessful</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="11" t="str">
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 5.25</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="11" t="str">
+      <c r="F26" s="26"/>
+      <c r="G26" s="25" t="str">
         <f>"Overall Grade : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade : C</v>
       </c>
-      <c r="H26" s="12"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="7" t="str">
         <f>"Range : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range : 55-59.99</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15" t="str">
+      <c r="B27" s="30"/>
+      <c r="C27" s="30" t="str">
         <f>'[2]Subjects List'!$C$15</f>
         <v>10/02/2019</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28"/>
@@ -29822,19 +29822,19 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E31"/>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
@@ -29848,41 +29848,63 @@
       <c r="D33"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="6uDjkxwoVLh/5XkJynEzWUewT4HJEkkxidDAMqElm8OVDscFoGN/6rfc2+Kpz3LVPElR4FPYGS6liUrrj9h5GA==" saltValue="kvKU5LSY2+e0GjmsTVlh0Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="D13" name="Seat No."/>
   </protectedRanges>
   <mergeCells count="37">
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A1:I6"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="A35:I35"/>
     <mergeCell ref="A9:G9"/>
@@ -29899,27 +29921,6 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="D32:F32"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A1:I6"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.69" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sem 2 Updated to v3
Sem 2 Updated to v3
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/Grade Card - Open.xlsx
+++ b/Batch 2018-20/Sem 1/Grade Card - Open.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B71E0EE-9F9F-4916-86D6-0E3D8B47281F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6D057F-4AE8-4BB5-BF1A-664DA33C0495}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>University of Mumbai</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Course Title</t>
   </si>
@@ -104,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,24 +118,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Old English Text MT"/>
-      <family val="4"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Old English Text MT"/>
-      <family val="4"/>
     </font>
     <font>
       <sz val="10"/>
@@ -279,105 +264,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,7 +405,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2146"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2149"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -477,16 +456,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1126625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0495B52-70FF-4F9D-9FC7-EEF95A442166}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8BBE401-F5D8-4CF6-853F-08DF4CC5FEF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -495,7 +474,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -509,7 +488,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5746750" cy="1619250"/>
+          <a:ext cx="5778000" cy="1969200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2098,7 +2077,7 @@
             <v>70</v>
           </cell>
           <cell r="T3" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U3" t="str">
             <v>8</v>
@@ -2110,25 +2089,25 @@
             <v>32</v>
           </cell>
           <cell r="X3">
-            <v>30</v>
+            <v>28</v>
           </cell>
           <cell r="Y3">
-            <v>40</v>
+            <v>37</v>
           </cell>
           <cell r="Z3">
-            <v>70</v>
+            <v>65</v>
           </cell>
           <cell r="AA3" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="AB3" t="str">
-            <v>8</v>
+            <v>7</v>
           </cell>
           <cell r="AC3">
             <v>4</v>
           </cell>
           <cell r="AD3">
-            <v>32</v>
+            <v>28</v>
           </cell>
           <cell r="AE3">
             <v>30</v>
@@ -2215,28 +2194,28 @@
             <v>32</v>
           </cell>
           <cell r="BG3">
-            <v>228</v>
+            <v>226</v>
           </cell>
           <cell r="BH3">
-            <v>356</v>
+            <v>353</v>
           </cell>
           <cell r="BI3">
-            <v>584</v>
+            <v>579</v>
           </cell>
           <cell r="BJ3">
-            <v>66</v>
+            <v>65</v>
           </cell>
           <cell r="BK3">
-            <v>264</v>
+            <v>260</v>
           </cell>
           <cell r="BL3">
-            <v>73</v>
+            <v>73.75</v>
           </cell>
           <cell r="BM3" t="str">
             <v>Unsuccessful</v>
           </cell>
           <cell r="BN3">
-            <v>8.25</v>
+            <v>8.125</v>
           </cell>
           <cell r="BO3" t="str">
             <v>A</v>
@@ -2304,7 +2283,7 @@
             <v>60</v>
           </cell>
           <cell r="T4" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U4" t="str">
             <v>6</v>
@@ -2436,7 +2415,7 @@
             <v>168</v>
           </cell>
           <cell r="BL4">
-            <v>58.5</v>
+            <v>45</v>
           </cell>
           <cell r="BM4" t="str">
             <v>Unsuccessful</v>
@@ -2510,7 +2489,7 @@
             <v>74</v>
           </cell>
           <cell r="T5" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U5" t="str">
             <v>8</v>
@@ -2642,7 +2621,7 @@
             <v>240</v>
           </cell>
           <cell r="BL5">
-            <v>71.25</v>
+            <v>67.5</v>
           </cell>
           <cell r="BM5" t="str">
             <v>Unsuccessful</v>
@@ -2651,7 +2630,7 @@
             <v>7.5</v>
           </cell>
           <cell r="BO5" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="BP5" t="str">
             <v>65-69.99</v>
@@ -2848,7 +2827,7 @@
             <v>284</v>
           </cell>
           <cell r="BL6">
-            <v>75.5</v>
+            <v>81.25</v>
           </cell>
           <cell r="BM6" t="str">
             <v>Successful</v>
@@ -2922,7 +2901,7 @@
             <v>69</v>
           </cell>
           <cell r="T7" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U7" t="str">
             <v>7</v>
@@ -3054,7 +3033,7 @@
             <v>224</v>
           </cell>
           <cell r="BL7">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM7" t="str">
             <v>Successful</v>
@@ -3128,7 +3107,7 @@
             <v>71</v>
           </cell>
           <cell r="T8" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U8" t="str">
             <v>8</v>
@@ -3260,7 +3239,7 @@
             <v>256</v>
           </cell>
           <cell r="BL8">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM8" t="str">
             <v>Successful</v>
@@ -3334,7 +3313,7 @@
             <v>71</v>
           </cell>
           <cell r="T9" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U9" t="str">
             <v>8</v>
@@ -3466,7 +3445,7 @@
             <v>256</v>
           </cell>
           <cell r="BL9">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM9" t="str">
             <v>Successful</v>
@@ -3672,7 +3651,7 @@
             <v>288</v>
           </cell>
           <cell r="BL10">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM10" t="str">
             <v>Successful</v>
@@ -3746,7 +3725,7 @@
             <v>67</v>
           </cell>
           <cell r="T11" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U11" t="str">
             <v>7</v>
@@ -3878,7 +3857,7 @@
             <v>224</v>
           </cell>
           <cell r="BL11">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM11" t="str">
             <v>Successful</v>
@@ -3952,7 +3931,7 @@
             <v>69</v>
           </cell>
           <cell r="T12" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U12" t="str">
             <v>7</v>
@@ -4084,7 +4063,7 @@
             <v>224</v>
           </cell>
           <cell r="BL12">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM12" t="str">
             <v>Successful</v>
@@ -4158,7 +4137,7 @@
             <v>65</v>
           </cell>
           <cell r="T13" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U13" t="str">
             <v>7</v>
@@ -4290,7 +4269,7 @@
             <v>224</v>
           </cell>
           <cell r="BL13">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM13" t="str">
             <v>Successful</v>
@@ -4364,7 +4343,7 @@
             <v>70</v>
           </cell>
           <cell r="T14" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U14" t="str">
             <v>8</v>
@@ -4496,7 +4475,7 @@
             <v>256</v>
           </cell>
           <cell r="BL14">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM14" t="str">
             <v>Successful</v>
@@ -4570,7 +4549,7 @@
             <v>60</v>
           </cell>
           <cell r="T15" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U15" t="str">
             <v>6</v>
@@ -4702,7 +4681,7 @@
             <v>192</v>
           </cell>
           <cell r="BL15">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM15" t="str">
             <v>Successful</v>
@@ -4776,7 +4755,7 @@
             <v>74</v>
           </cell>
           <cell r="T16" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U16" t="str">
             <v>8</v>
@@ -4908,7 +4887,7 @@
             <v>256</v>
           </cell>
           <cell r="BL16">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM16" t="str">
             <v>Successful</v>
@@ -5114,7 +5093,7 @@
             <v>288</v>
           </cell>
           <cell r="BL17">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM17" t="str">
             <v>Successful</v>
@@ -5188,7 +5167,7 @@
             <v>69</v>
           </cell>
           <cell r="T18" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U18" t="str">
             <v>7</v>
@@ -5320,7 +5299,7 @@
             <v>224</v>
           </cell>
           <cell r="BL18">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM18" t="str">
             <v>Successful</v>
@@ -5394,7 +5373,7 @@
             <v>71</v>
           </cell>
           <cell r="T19" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U19" t="str">
             <v>8</v>
@@ -5526,7 +5505,7 @@
             <v>256</v>
           </cell>
           <cell r="BL19">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM19" t="str">
             <v>Successful</v>
@@ -5600,7 +5579,7 @@
             <v>71</v>
           </cell>
           <cell r="T20" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U20" t="str">
             <v>8</v>
@@ -5732,7 +5711,7 @@
             <v>256</v>
           </cell>
           <cell r="BL20">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM20" t="str">
             <v>Successful</v>
@@ -5938,7 +5917,7 @@
             <v>288</v>
           </cell>
           <cell r="BL21">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM21" t="str">
             <v>Successful</v>
@@ -6012,7 +5991,7 @@
             <v>67</v>
           </cell>
           <cell r="T22" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U22" t="str">
             <v>7</v>
@@ -6144,7 +6123,7 @@
             <v>224</v>
           </cell>
           <cell r="BL22">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM22" t="str">
             <v>Successful</v>
@@ -6218,7 +6197,7 @@
             <v>69</v>
           </cell>
           <cell r="T23" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U23" t="str">
             <v>7</v>
@@ -6350,7 +6329,7 @@
             <v>224</v>
           </cell>
           <cell r="BL23">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM23" t="str">
             <v>Successful</v>
@@ -6556,7 +6535,7 @@
             <v>0</v>
           </cell>
           <cell r="BL24">
-            <v>0</v>
+            <v>-7.5</v>
           </cell>
           <cell r="BM24" t="str">
             <v>Unsuccessful</v>
@@ -6630,7 +6609,7 @@
             <v>70</v>
           </cell>
           <cell r="T25" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U25" t="str">
             <v>8</v>
@@ -6762,7 +6741,7 @@
             <v>256</v>
           </cell>
           <cell r="BL25">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM25" t="str">
             <v>Successful</v>
@@ -6836,7 +6815,7 @@
             <v>60</v>
           </cell>
           <cell r="T26" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U26" t="str">
             <v>6</v>
@@ -6968,7 +6947,7 @@
             <v>192</v>
           </cell>
           <cell r="BL26">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM26" t="str">
             <v>Successful</v>
@@ -7042,7 +7021,7 @@
             <v>74</v>
           </cell>
           <cell r="T27" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U27" t="str">
             <v>8</v>
@@ -7174,7 +7153,7 @@
             <v>256</v>
           </cell>
           <cell r="BL27">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM27" t="str">
             <v>Successful</v>
@@ -7380,7 +7359,7 @@
             <v>288</v>
           </cell>
           <cell r="BL28">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM28" t="str">
             <v>Successful</v>
@@ -7454,7 +7433,7 @@
             <v>69</v>
           </cell>
           <cell r="T29" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U29" t="str">
             <v>7</v>
@@ -7586,7 +7565,7 @@
             <v>224</v>
           </cell>
           <cell r="BL29">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM29" t="str">
             <v>Successful</v>
@@ -7660,7 +7639,7 @@
             <v>71</v>
           </cell>
           <cell r="T30" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U30" t="str">
             <v>8</v>
@@ -7792,7 +7771,7 @@
             <v>256</v>
           </cell>
           <cell r="BL30">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM30" t="str">
             <v>Successful</v>
@@ -7866,7 +7845,7 @@
             <v>71</v>
           </cell>
           <cell r="T31" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U31" t="str">
             <v>8</v>
@@ -7998,7 +7977,7 @@
             <v>256</v>
           </cell>
           <cell r="BL31">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM31" t="str">
             <v>Successful</v>
@@ -8204,7 +8183,7 @@
             <v>288</v>
           </cell>
           <cell r="BL32">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM32" t="str">
             <v>Successful</v>
@@ -8278,7 +8257,7 @@
             <v>67</v>
           </cell>
           <cell r="T33" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U33" t="str">
             <v>7</v>
@@ -8410,7 +8389,7 @@
             <v>224</v>
           </cell>
           <cell r="BL33">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM33" t="str">
             <v>Successful</v>
@@ -8484,7 +8463,7 @@
             <v>69</v>
           </cell>
           <cell r="T34" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U34" t="str">
             <v>7</v>
@@ -8616,7 +8595,7 @@
             <v>224</v>
           </cell>
           <cell r="BL34">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM34" t="str">
             <v>Successful</v>
@@ -8690,7 +8669,7 @@
             <v>65</v>
           </cell>
           <cell r="T35" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U35" t="str">
             <v>7</v>
@@ -8822,7 +8801,7 @@
             <v>224</v>
           </cell>
           <cell r="BL35">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM35" t="str">
             <v>Successful</v>
@@ -8896,7 +8875,7 @@
             <v>70</v>
           </cell>
           <cell r="T36" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U36" t="str">
             <v>8</v>
@@ -9028,7 +9007,7 @@
             <v>256</v>
           </cell>
           <cell r="BL36">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM36" t="str">
             <v>Successful</v>
@@ -9102,7 +9081,7 @@
             <v>60</v>
           </cell>
           <cell r="T37" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U37" t="str">
             <v>6</v>
@@ -9234,7 +9213,7 @@
             <v>192</v>
           </cell>
           <cell r="BL37">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM37" t="str">
             <v>Successful</v>
@@ -9308,7 +9287,7 @@
             <v>74</v>
           </cell>
           <cell r="T38" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U38" t="str">
             <v>8</v>
@@ -9440,7 +9419,7 @@
             <v>256</v>
           </cell>
           <cell r="BL38">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM38" t="str">
             <v>Successful</v>
@@ -9646,7 +9625,7 @@
             <v>288</v>
           </cell>
           <cell r="BL39">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM39" t="str">
             <v>Successful</v>
@@ -9720,7 +9699,7 @@
             <v>69</v>
           </cell>
           <cell r="T40" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U40" t="str">
             <v>7</v>
@@ -9852,7 +9831,7 @@
             <v>224</v>
           </cell>
           <cell r="BL40">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM40" t="str">
             <v>Successful</v>
@@ -9926,7 +9905,7 @@
             <v>71</v>
           </cell>
           <cell r="T41" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U41" t="str">
             <v>8</v>
@@ -10058,7 +10037,7 @@
             <v>256</v>
           </cell>
           <cell r="BL41">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM41" t="str">
             <v>Successful</v>
@@ -10132,7 +10111,7 @@
             <v>71</v>
           </cell>
           <cell r="T42" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U42" t="str">
             <v>8</v>
@@ -10264,7 +10243,7 @@
             <v>256</v>
           </cell>
           <cell r="BL42">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM42" t="str">
             <v>Successful</v>
@@ -10470,7 +10449,7 @@
             <v>288</v>
           </cell>
           <cell r="BL43">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM43" t="str">
             <v>Successful</v>
@@ -10544,7 +10523,7 @@
             <v>67</v>
           </cell>
           <cell r="T44" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U44" t="str">
             <v>7</v>
@@ -10676,7 +10655,7 @@
             <v>224</v>
           </cell>
           <cell r="BL44">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM44" t="str">
             <v>Successful</v>
@@ -10882,7 +10861,7 @@
             <v>0</v>
           </cell>
           <cell r="BL45">
-            <v>0</v>
+            <v>-7.5</v>
           </cell>
           <cell r="BM45" t="str">
             <v>Unsuccessful</v>
@@ -10956,7 +10935,7 @@
             <v>65</v>
           </cell>
           <cell r="T46" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U46" t="str">
             <v>7</v>
@@ -11088,7 +11067,7 @@
             <v>224</v>
           </cell>
           <cell r="BL46">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM46" t="str">
             <v>Successful</v>
@@ -11162,7 +11141,7 @@
             <v>70</v>
           </cell>
           <cell r="T47" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U47" t="str">
             <v>8</v>
@@ -11294,7 +11273,7 @@
             <v>256</v>
           </cell>
           <cell r="BL47">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM47" t="str">
             <v>Successful</v>
@@ -11368,7 +11347,7 @@
             <v>60</v>
           </cell>
           <cell r="T48" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U48" t="str">
             <v>6</v>
@@ -11500,7 +11479,7 @@
             <v>192</v>
           </cell>
           <cell r="BL48">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM48" t="str">
             <v>Successful</v>
@@ -11574,7 +11553,7 @@
             <v>74</v>
           </cell>
           <cell r="T49" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U49" t="str">
             <v>8</v>
@@ -11706,7 +11685,7 @@
             <v>256</v>
           </cell>
           <cell r="BL49">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM49" t="str">
             <v>Successful</v>
@@ -11912,7 +11891,7 @@
             <v>288</v>
           </cell>
           <cell r="BL50">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM50" t="str">
             <v>Successful</v>
@@ -11986,7 +11965,7 @@
             <v>69</v>
           </cell>
           <cell r="T51" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U51" t="str">
             <v>7</v>
@@ -12118,7 +12097,7 @@
             <v>224</v>
           </cell>
           <cell r="BL51">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM51" t="str">
             <v>Successful</v>
@@ -12192,7 +12171,7 @@
             <v>71</v>
           </cell>
           <cell r="T52" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U52" t="str">
             <v>8</v>
@@ -12324,7 +12303,7 @@
             <v>256</v>
           </cell>
           <cell r="BL52">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM52" t="str">
             <v>Successful</v>
@@ -12398,7 +12377,7 @@
             <v>71</v>
           </cell>
           <cell r="T53" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U53" t="str">
             <v>8</v>
@@ -12530,7 +12509,7 @@
             <v>256</v>
           </cell>
           <cell r="BL53">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM53" t="str">
             <v>Successful</v>
@@ -12736,7 +12715,7 @@
             <v>288</v>
           </cell>
           <cell r="BL54">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM54" t="str">
             <v>Successful</v>
@@ -12810,7 +12789,7 @@
             <v>67</v>
           </cell>
           <cell r="T55" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U55" t="str">
             <v>7</v>
@@ -12942,7 +12921,7 @@
             <v>224</v>
           </cell>
           <cell r="BL55">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM55" t="str">
             <v>Successful</v>
@@ -13016,7 +12995,7 @@
             <v>69</v>
           </cell>
           <cell r="T56" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U56" t="str">
             <v>7</v>
@@ -13148,7 +13127,7 @@
             <v>224</v>
           </cell>
           <cell r="BL56">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM56" t="str">
             <v>Successful</v>
@@ -13222,7 +13201,7 @@
             <v>65</v>
           </cell>
           <cell r="T57" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U57" t="str">
             <v>7</v>
@@ -13354,7 +13333,7 @@
             <v>224</v>
           </cell>
           <cell r="BL57">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM57" t="str">
             <v>Successful</v>
@@ -13428,7 +13407,7 @@
             <v>70</v>
           </cell>
           <cell r="T58" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U58" t="str">
             <v>8</v>
@@ -13560,7 +13539,7 @@
             <v>256</v>
           </cell>
           <cell r="BL58">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM58" t="str">
             <v>Successful</v>
@@ -13634,7 +13613,7 @@
             <v>60</v>
           </cell>
           <cell r="T59" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U59" t="str">
             <v>6</v>
@@ -13766,7 +13745,7 @@
             <v>192</v>
           </cell>
           <cell r="BL59">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM59" t="str">
             <v>Successful</v>
@@ -13840,7 +13819,7 @@
             <v>74</v>
           </cell>
           <cell r="T60" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U60" t="str">
             <v>8</v>
@@ -13972,7 +13951,7 @@
             <v>256</v>
           </cell>
           <cell r="BL60">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM60" t="str">
             <v>Successful</v>
@@ -14178,7 +14157,7 @@
             <v>288</v>
           </cell>
           <cell r="BL61">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM61" t="str">
             <v>Successful</v>
@@ -14252,7 +14231,7 @@
             <v>69</v>
           </cell>
           <cell r="T62" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U62" t="str">
             <v>7</v>
@@ -14384,7 +14363,7 @@
             <v>224</v>
           </cell>
           <cell r="BL62">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM62" t="str">
             <v>Successful</v>
@@ -14458,7 +14437,7 @@
             <v>71</v>
           </cell>
           <cell r="T63" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U63" t="str">
             <v>8</v>
@@ -14590,7 +14569,7 @@
             <v>256</v>
           </cell>
           <cell r="BL63">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM63" t="str">
             <v>Successful</v>
@@ -14664,7 +14643,7 @@
             <v>71</v>
           </cell>
           <cell r="T64" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U64" t="str">
             <v>8</v>
@@ -14796,7 +14775,7 @@
             <v>256</v>
           </cell>
           <cell r="BL64">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM64" t="str">
             <v>Successful</v>
@@ -15002,7 +14981,7 @@
             <v>288</v>
           </cell>
           <cell r="BL65">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM65" t="str">
             <v>Successful</v>
@@ -15076,7 +15055,7 @@
             <v>67</v>
           </cell>
           <cell r="T66" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U66" t="str">
             <v>7</v>
@@ -15208,7 +15187,7 @@
             <v>224</v>
           </cell>
           <cell r="BL66">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM66" t="str">
             <v>Successful</v>
@@ -15282,7 +15261,7 @@
             <v>69</v>
           </cell>
           <cell r="T67" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U67" t="str">
             <v>7</v>
@@ -15414,7 +15393,7 @@
             <v>224</v>
           </cell>
           <cell r="BL67">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM67" t="str">
             <v>Successful</v>
@@ -15488,7 +15467,7 @@
             <v>65</v>
           </cell>
           <cell r="T68" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U68" t="str">
             <v>7</v>
@@ -15620,7 +15599,7 @@
             <v>224</v>
           </cell>
           <cell r="BL68">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM68" t="str">
             <v>Successful</v>
@@ -15694,7 +15673,7 @@
             <v>70</v>
           </cell>
           <cell r="T69" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U69" t="str">
             <v>8</v>
@@ -15826,7 +15805,7 @@
             <v>256</v>
           </cell>
           <cell r="BL69">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM69" t="str">
             <v>Successful</v>
@@ -15900,7 +15879,7 @@
             <v>60</v>
           </cell>
           <cell r="T70" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U70" t="str">
             <v>6</v>
@@ -16032,7 +16011,7 @@
             <v>192</v>
           </cell>
           <cell r="BL70">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM70" t="str">
             <v>Successful</v>
@@ -16106,7 +16085,7 @@
             <v>74</v>
           </cell>
           <cell r="T71" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U71" t="str">
             <v>8</v>
@@ -16238,7 +16217,7 @@
             <v>256</v>
           </cell>
           <cell r="BL71">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM71" t="str">
             <v>Successful</v>
@@ -16444,7 +16423,7 @@
             <v>288</v>
           </cell>
           <cell r="BL72">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM72" t="str">
             <v>Successful</v>
@@ -16518,7 +16497,7 @@
             <v>69</v>
           </cell>
           <cell r="T73" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U73" t="str">
             <v>7</v>
@@ -16650,7 +16629,7 @@
             <v>224</v>
           </cell>
           <cell r="BL73">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM73" t="str">
             <v>Successful</v>
@@ -16724,7 +16703,7 @@
             <v>71</v>
           </cell>
           <cell r="T74" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U74" t="str">
             <v>8</v>
@@ -16856,7 +16835,7 @@
             <v>256</v>
           </cell>
           <cell r="BL74">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM74" t="str">
             <v>Successful</v>
@@ -16930,7 +16909,7 @@
             <v>71</v>
           </cell>
           <cell r="T75" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U75" t="str">
             <v>8</v>
@@ -17062,7 +17041,7 @@
             <v>256</v>
           </cell>
           <cell r="BL75">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM75" t="str">
             <v>Successful</v>
@@ -17268,7 +17247,7 @@
             <v>288</v>
           </cell>
           <cell r="BL76">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM76" t="str">
             <v>Successful</v>
@@ -17342,7 +17321,7 @@
             <v>67</v>
           </cell>
           <cell r="T77" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U77" t="str">
             <v>7</v>
@@ -17474,7 +17453,7 @@
             <v>224</v>
           </cell>
           <cell r="BL77">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM77" t="str">
             <v>Successful</v>
@@ -17548,7 +17527,7 @@
             <v>69</v>
           </cell>
           <cell r="T78" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U78" t="str">
             <v>7</v>
@@ -17680,7 +17659,7 @@
             <v>224</v>
           </cell>
           <cell r="BL78">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM78" t="str">
             <v>Successful</v>
@@ -17754,7 +17733,7 @@
             <v>65</v>
           </cell>
           <cell r="T79" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U79" t="str">
             <v>7</v>
@@ -17886,7 +17865,7 @@
             <v>224</v>
           </cell>
           <cell r="BL79">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM79" t="str">
             <v>Successful</v>
@@ -17960,7 +17939,7 @@
             <v>70</v>
           </cell>
           <cell r="T80" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U80" t="str">
             <v>8</v>
@@ -18092,7 +18071,7 @@
             <v>256</v>
           </cell>
           <cell r="BL80">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM80" t="str">
             <v>Successful</v>
@@ -18166,7 +18145,7 @@
             <v>60</v>
           </cell>
           <cell r="T81" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U81" t="str">
             <v>6</v>
@@ -18298,7 +18277,7 @@
             <v>192</v>
           </cell>
           <cell r="BL81">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM81" t="str">
             <v>Successful</v>
@@ -18372,7 +18351,7 @@
             <v>74</v>
           </cell>
           <cell r="T82" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U82" t="str">
             <v>8</v>
@@ -18504,7 +18483,7 @@
             <v>256</v>
           </cell>
           <cell r="BL82">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM82" t="str">
             <v>Successful</v>
@@ -18710,7 +18689,7 @@
             <v>288</v>
           </cell>
           <cell r="BL83">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM83" t="str">
             <v>Successful</v>
@@ -18784,7 +18763,7 @@
             <v>69</v>
           </cell>
           <cell r="T84" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U84" t="str">
             <v>7</v>
@@ -18916,7 +18895,7 @@
             <v>224</v>
           </cell>
           <cell r="BL84">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM84" t="str">
             <v>Successful</v>
@@ -18990,7 +18969,7 @@
             <v>71</v>
           </cell>
           <cell r="T85" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U85" t="str">
             <v>8</v>
@@ -19122,7 +19101,7 @@
             <v>256</v>
           </cell>
           <cell r="BL85">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM85" t="str">
             <v>Successful</v>
@@ -19196,7 +19175,7 @@
             <v>71</v>
           </cell>
           <cell r="T86" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U86" t="str">
             <v>8</v>
@@ -19328,7 +19307,7 @@
             <v>256</v>
           </cell>
           <cell r="BL86">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM86" t="str">
             <v>Successful</v>
@@ -19534,7 +19513,7 @@
             <v>288</v>
           </cell>
           <cell r="BL87">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM87" t="str">
             <v>Successful</v>
@@ -19608,7 +19587,7 @@
             <v>67</v>
           </cell>
           <cell r="T88" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U88" t="str">
             <v>7</v>
@@ -19740,7 +19719,7 @@
             <v>224</v>
           </cell>
           <cell r="BL88">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM88" t="str">
             <v>Successful</v>
@@ -19814,7 +19793,7 @@
             <v>69</v>
           </cell>
           <cell r="T89" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U89" t="str">
             <v>7</v>
@@ -19946,7 +19925,7 @@
             <v>224</v>
           </cell>
           <cell r="BL89">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM89" t="str">
             <v>Successful</v>
@@ -20020,7 +19999,7 @@
             <v>65</v>
           </cell>
           <cell r="T90" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U90" t="str">
             <v>7</v>
@@ -20152,7 +20131,7 @@
             <v>224</v>
           </cell>
           <cell r="BL90">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM90" t="str">
             <v>Successful</v>
@@ -20226,7 +20205,7 @@
             <v>70</v>
           </cell>
           <cell r="T91" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U91" t="str">
             <v>8</v>
@@ -20358,7 +20337,7 @@
             <v>256</v>
           </cell>
           <cell r="BL91">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM91" t="str">
             <v>Successful</v>
@@ -20432,7 +20411,7 @@
             <v>60</v>
           </cell>
           <cell r="T92" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U92" t="str">
             <v>6</v>
@@ -20564,7 +20543,7 @@
             <v>192</v>
           </cell>
           <cell r="BL92">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM92" t="str">
             <v>Successful</v>
@@ -20638,7 +20617,7 @@
             <v>74</v>
           </cell>
           <cell r="T93" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U93" t="str">
             <v>8</v>
@@ -20770,7 +20749,7 @@
             <v>256</v>
           </cell>
           <cell r="BL93">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM93" t="str">
             <v>Successful</v>
@@ -20976,7 +20955,7 @@
             <v>288</v>
           </cell>
           <cell r="BL94">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM94" t="str">
             <v>Successful</v>
@@ -21050,7 +21029,7 @@
             <v>69</v>
           </cell>
           <cell r="T95" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U95" t="str">
             <v>7</v>
@@ -21182,7 +21161,7 @@
             <v>224</v>
           </cell>
           <cell r="BL95">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM95" t="str">
             <v>Successful</v>
@@ -21256,7 +21235,7 @@
             <v>71</v>
           </cell>
           <cell r="T96" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U96" t="str">
             <v>8</v>
@@ -21388,7 +21367,7 @@
             <v>256</v>
           </cell>
           <cell r="BL96">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM96" t="str">
             <v>Successful</v>
@@ -21462,7 +21441,7 @@
             <v>71</v>
           </cell>
           <cell r="T97" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U97" t="str">
             <v>8</v>
@@ -21594,7 +21573,7 @@
             <v>256</v>
           </cell>
           <cell r="BL97">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM97" t="str">
             <v>Successful</v>
@@ -21800,7 +21779,7 @@
             <v>288</v>
           </cell>
           <cell r="BL98">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM98" t="str">
             <v>Successful</v>
@@ -21874,7 +21853,7 @@
             <v>67</v>
           </cell>
           <cell r="T99" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U99" t="str">
             <v>7</v>
@@ -22006,7 +21985,7 @@
             <v>224</v>
           </cell>
           <cell r="BL99">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM99" t="str">
             <v>Successful</v>
@@ -22080,7 +22059,7 @@
             <v>69</v>
           </cell>
           <cell r="T100" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U100" t="str">
             <v>7</v>
@@ -22212,7 +22191,7 @@
             <v>224</v>
           </cell>
           <cell r="BL100">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM100" t="str">
             <v>Successful</v>
@@ -22286,7 +22265,7 @@
             <v>65</v>
           </cell>
           <cell r="T101" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U101" t="str">
             <v>7</v>
@@ -22418,7 +22397,7 @@
             <v>224</v>
           </cell>
           <cell r="BL101">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM101" t="str">
             <v>Successful</v>
@@ -22492,7 +22471,7 @@
             <v>70</v>
           </cell>
           <cell r="T102" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U102" t="str">
             <v>8</v>
@@ -22624,7 +22603,7 @@
             <v>256</v>
           </cell>
           <cell r="BL102">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM102" t="str">
             <v>Successful</v>
@@ -22698,7 +22677,7 @@
             <v>60</v>
           </cell>
           <cell r="T103" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U103" t="str">
             <v>6</v>
@@ -22830,7 +22809,7 @@
             <v>192</v>
           </cell>
           <cell r="BL103">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM103" t="str">
             <v>Successful</v>
@@ -22904,7 +22883,7 @@
             <v>74</v>
           </cell>
           <cell r="T104" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U104" t="str">
             <v>8</v>
@@ -23036,7 +23015,7 @@
             <v>256</v>
           </cell>
           <cell r="BL104">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM104" t="str">
             <v>Successful</v>
@@ -23242,7 +23221,7 @@
             <v>288</v>
           </cell>
           <cell r="BL105">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM105" t="str">
             <v>Successful</v>
@@ -23316,7 +23295,7 @@
             <v>69</v>
           </cell>
           <cell r="T106" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U106" t="str">
             <v>7</v>
@@ -23448,7 +23427,7 @@
             <v>224</v>
           </cell>
           <cell r="BL106">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM106" t="str">
             <v>Successful</v>
@@ -23522,7 +23501,7 @@
             <v>71</v>
           </cell>
           <cell r="T107" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U107" t="str">
             <v>8</v>
@@ -23654,7 +23633,7 @@
             <v>256</v>
           </cell>
           <cell r="BL107">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM107" t="str">
             <v>Successful</v>
@@ -23728,7 +23707,7 @@
             <v>71</v>
           </cell>
           <cell r="T108" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U108" t="str">
             <v>8</v>
@@ -23860,7 +23839,7 @@
             <v>256</v>
           </cell>
           <cell r="BL108">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM108" t="str">
             <v>Successful</v>
@@ -24066,7 +24045,7 @@
             <v>288</v>
           </cell>
           <cell r="BL109">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM109" t="str">
             <v>Successful</v>
@@ -24140,7 +24119,7 @@
             <v>67</v>
           </cell>
           <cell r="T110" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U110" t="str">
             <v>7</v>
@@ -24272,7 +24251,7 @@
             <v>224</v>
           </cell>
           <cell r="BL110">
-            <v>67</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM110" t="str">
             <v>Successful</v>
@@ -24346,7 +24325,7 @@
             <v>69</v>
           </cell>
           <cell r="T111" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U111" t="str">
             <v>7</v>
@@ -24478,7 +24457,7 @@
             <v>224</v>
           </cell>
           <cell r="BL111">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM111" t="str">
             <v>Successful</v>
@@ -24552,7 +24531,7 @@
             <v>65</v>
           </cell>
           <cell r="T112" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U112" t="str">
             <v>7</v>
@@ -24684,7 +24663,7 @@
             <v>224</v>
           </cell>
           <cell r="BL112">
-            <v>65</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM112" t="str">
             <v>Successful</v>
@@ -24758,7 +24737,7 @@
             <v>70</v>
           </cell>
           <cell r="T113" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U113" t="str">
             <v>8</v>
@@ -24890,7 +24869,7 @@
             <v>256</v>
           </cell>
           <cell r="BL113">
-            <v>70</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM113" t="str">
             <v>Successful</v>
@@ -24964,7 +24943,7 @@
             <v>60</v>
           </cell>
           <cell r="T114" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U114" t="str">
             <v>6</v>
@@ -25096,7 +25075,7 @@
             <v>192</v>
           </cell>
           <cell r="BL114">
-            <v>60</v>
+            <v>52.5</v>
           </cell>
           <cell r="BM114" t="str">
             <v>Successful</v>
@@ -25170,7 +25149,7 @@
             <v>74</v>
           </cell>
           <cell r="T115" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U115" t="str">
             <v>8</v>
@@ -25302,7 +25281,7 @@
             <v>256</v>
           </cell>
           <cell r="BL115">
-            <v>74</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM115" t="str">
             <v>Successful</v>
@@ -25508,7 +25487,7 @@
             <v>288</v>
           </cell>
           <cell r="BL116">
-            <v>76</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM116" t="str">
             <v>Successful</v>
@@ -25582,7 +25561,7 @@
             <v>69</v>
           </cell>
           <cell r="T117" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U117" t="str">
             <v>7</v>
@@ -25714,7 +25693,7 @@
             <v>224</v>
           </cell>
           <cell r="BL117">
-            <v>69</v>
+            <v>62.5</v>
           </cell>
           <cell r="BM117" t="str">
             <v>Successful</v>
@@ -25788,7 +25767,7 @@
             <v>71</v>
           </cell>
           <cell r="T118" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U118" t="str">
             <v>8</v>
@@ -25920,7 +25899,7 @@
             <v>256</v>
           </cell>
           <cell r="BL118">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM118" t="str">
             <v>Successful</v>
@@ -25994,7 +25973,7 @@
             <v>71</v>
           </cell>
           <cell r="T119" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U119" t="str">
             <v>8</v>
@@ -26126,7 +26105,7 @@
             <v>256</v>
           </cell>
           <cell r="BL119">
-            <v>71</v>
+            <v>72.5</v>
           </cell>
           <cell r="BM119" t="str">
             <v>Successful</v>
@@ -26332,7 +26311,7 @@
             <v>288</v>
           </cell>
           <cell r="BL120">
-            <v>75</v>
+            <v>82.5</v>
           </cell>
           <cell r="BM120" t="str">
             <v>Successful</v>
@@ -26406,7 +26385,7 @@
             <v>67</v>
           </cell>
           <cell r="T121" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U121" t="str">
             <v>7</v>
@@ -26538,7 +26517,7 @@
             <v>220</v>
           </cell>
           <cell r="BL121">
-            <v>66.5</v>
+            <v>61.25</v>
           </cell>
           <cell r="BM121" t="str">
             <v>Successful</v>
@@ -26744,7 +26723,7 @@
             <v>0</v>
           </cell>
           <cell r="BL122">
-            <v>0</v>
+            <v>-7.5</v>
           </cell>
           <cell r="BM122" t="str">
             <v>Unsuccessful</v>
@@ -29275,7 +29254,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I6"/>
+      <selection sqref="A1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29293,221 +29272,219 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
+    <row r="7" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="str">
+      <c r="A9" s="13" t="str">
         <f>"NAME OF THE CANDIDATE : "&amp;VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>NAME OF THE CANDIDATE : /ADIVAREKAR PRITI GIRIGHAR NAMRATA</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
+      <c r="A10" s="13" t="s">
+        <v>13</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="str">
+      <c r="A11" s="13" t="str">
         <f>"HELD IN : "&amp;'[2]Subjects List'!$C$13</f>
         <v>HELD IN : JANUARY 2019</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>15</v>
+      <c r="A12" s="13" t="s">
+        <v>14</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>9</v>
+      <c r="A13" s="13" t="s">
+        <v>8</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>18</v>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>17</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14" t="s">
+      <c r="F15" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>4</v>
+      <c r="G15" s="19" t="s">
+        <v>9</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>5</v>
+      <c r="I15" s="19" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="16" t="str">
+      <c r="B17" s="18" t="str">
         <f>'[2]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="3">
         <v>4</v>
       </c>
@@ -29531,12 +29508,12 @@
       <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="16" t="str">
+      <c r="B18" s="18" t="str">
         <f>'[2]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="3">
         <v>4</v>
       </c>
@@ -29560,18 +29537,18 @@
       <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="16" t="str">
+      <c r="B19" s="18" t="str">
         <f>'[2]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="3">
         <v>4</v>
       </c>
       <c r="F19" s="3" t="str">
         <f>VLOOKUP(D13,'[3]Subject Marks'!$A$3:$T$135,20,0)</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="G19" s="3">
         <v>4</v>
@@ -29589,12 +29566,12 @@
       <c r="A20" s="3">
         <v>4</v>
       </c>
-      <c r="B20" s="16" t="str">
+      <c r="B20" s="18" t="str">
         <f>'[2]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="3">
         <v>4</v>
       </c>
@@ -29618,12 +29595,12 @@
       <c r="A21" s="3">
         <v>5</v>
       </c>
-      <c r="B21" s="16" t="str">
+      <c r="B21" s="18" t="str">
         <f>'[2]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="3">
         <v>4</v>
       </c>
@@ -29647,12 +29624,12 @@
       <c r="A22" s="3">
         <v>6</v>
       </c>
-      <c r="B22" s="16" t="str">
+      <c r="B22" s="18" t="str">
         <f>'[2]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="3">
         <v>4</v>
       </c>
@@ -29676,12 +29653,12 @@
       <c r="A23" s="3">
         <v>7</v>
       </c>
-      <c r="B23" s="16" t="str">
+      <c r="B23" s="18" t="str">
         <f>'[2]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="3">
         <v>4</v>
       </c>
@@ -29705,12 +29682,12 @@
       <c r="A24" s="3">
         <v>8</v>
       </c>
-      <c r="B24" s="16" t="str">
+      <c r="B24" s="18" t="str">
         <f>'[2]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="3">
         <v>4</v>
       </c>
@@ -29732,11 +29709,11 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="17" t="s">
-        <v>7</v>
+      <c r="B25" s="29" t="s">
+        <v>6</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="5">
@@ -29757,36 +29734,36 @@
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
       <c r="D26" s="24"/>
-      <c r="E26" s="25" t="str">
+      <c r="E26" s="11" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 5.25</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="25" t="str">
+      <c r="F26" s="12"/>
+      <c r="G26" s="11" t="str">
         <f>"Overall Grade : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade : C</v>
       </c>
-      <c r="H26" s="26"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="7" t="str">
         <f>"Range : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range : 55-59.99</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>8</v>
+      <c r="A27" s="14" t="s">
+        <v>7</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30" t="str">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15" t="str">
         <f>'[2]Subjects List'!$C$15</f>
         <v>10/02/2019</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28"/>
@@ -29812,7 +29789,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30"/>
       <c r="C30" s="2"/>
@@ -29822,89 +29799,69 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E31"/>
-      <c r="G31" s="8" t="s">
-        <v>16</v>
+      <c r="G31" s="9" t="s">
+        <v>15</v>
       </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="8" t="s">
-        <v>17</v>
+      <c r="D34" s="9" t="s">
+        <v>16</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>6</v>
+      <c r="A38" s="8" t="s">
+        <v>5</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6uDjkxwoVLh/5XkJynEzWUewT4HJEkkxidDAMqElm8OVDscFoGN/6rfc2+Kpz3LVPElR4FPYGS6liUrrj9h5GA==" saltValue="kvKU5LSY2+e0GjmsTVlh0Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="x9S6RkJxY2uMsNbT4A3srL6TwSDcPlXgDKgVdPh7BOKRgw/BX1Ux/kn68m9NeXHF7ZIN+T9FHSxoTJbykBbf0Q==" saltValue="yKlTIDWS8mBnAYzrJCpM0w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="D13" name="Seat No."/>
   </protectedRanges>
-  <mergeCells count="37">
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A1:I6"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:F26"/>
+  <mergeCells count="36">
+    <mergeCell ref="A1:I7"/>
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="A35:I35"/>
     <mergeCell ref="A9:G9"/>
@@ -29921,6 +29878,25 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="D32:F32"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.69" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>